<commit_message>
Added buildingd to AG
</commit_message>
<xml_diff>
--- a/Pics/scale.xlsx
+++ b/Pics/scale.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ModelRRProjects\AnyRail\Pics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0-Data\AnyRail\Pics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F64755-960A-46C0-B5D9-C25F09E90836}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6BD9EF-D5BE-4E7E-82C2-33B55824F246}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39910" yWindow="20070" windowWidth="16710" windowHeight="10340" xr2:uid="{F2CF72A6-85D0-419B-8904-BB52EA359DE2}"/>
+    <workbookView xWindow="383" yWindow="405" windowWidth="23107" windowHeight="14055" xr2:uid="{F2CF72A6-85D0-419B-8904-BB52EA359DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>feet</t>
   </si>
@@ -64,6 +64,42 @@
   </si>
   <si>
     <t>Drying house</t>
+  </si>
+  <si>
+    <t>Coal Shed</t>
+  </si>
+  <si>
+    <t>EmissionsControl</t>
+  </si>
+  <si>
+    <t>Stacks on tower</t>
+  </si>
+  <si>
+    <t>heater</t>
+  </si>
+  <si>
+    <t>Bag house</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>Coal in</t>
+  </si>
+  <si>
+    <t>Klinker Crushing</t>
+  </si>
+  <si>
+    <t>Kiln exit</t>
+  </si>
+  <si>
+    <t>Old Bulk Loadout</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>Scale Height</t>
   </si>
 </sst>
 </file>
@@ -416,18 +452,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC5BF58-5D6E-4D62-AD7B-B2BB68C10829}">
-  <dimension ref="B3:G19"/>
+  <dimension ref="B3:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -440,8 +476,14 @@
       <c r="G3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -459,8 +501,15 @@
         <f>E4/2</f>
         <v>1.875</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>88</v>
+      </c>
+      <c r="K4">
+        <f>(J4/D4)*12</f>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -478,8 +527,15 @@
         <f t="shared" ref="G5:G19" si="1">E5/2</f>
         <v>1.6875</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>88</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K57" si="2">(J5/D5)*12</f>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -497,8 +553,15 @@
         <f t="shared" si="1"/>
         <v>10.875</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>88</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C7">
         <v>20</v>
       </c>
@@ -513,8 +576,15 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>88</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -532,8 +602,15 @@
         <f t="shared" si="1"/>
         <v>2.8125</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>88</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C9">
         <v>7</v>
       </c>
@@ -548,8 +625,15 @@
         <f t="shared" si="1"/>
         <v>0.26249999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>88</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C10">
         <v>68</v>
       </c>
@@ -564,8 +648,15 @@
         <f t="shared" si="1"/>
         <v>2.5499999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>88</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>48</v>
       </c>
@@ -580,8 +671,15 @@
         <f t="shared" si="1"/>
         <v>1.7999999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>88</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -599,8 +697,15 @@
         <f t="shared" si="1"/>
         <v>4.875</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>88</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>60</v>
       </c>
@@ -615,8 +720,15 @@
         <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>88</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -634,8 +746,15 @@
         <f t="shared" si="1"/>
         <v>1.5750000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>88</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -653,8 +772,15 @@
         <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>53</v>
       </c>
@@ -669,8 +795,15 @@
         <f t="shared" si="1"/>
         <v>1.9874999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>88</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>40</v>
       </c>
@@ -685,8 +818,15 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>88</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>25</v>
       </c>
@@ -701,21 +841,939 @@
         <f t="shared" si="1"/>
         <v>0.9375</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>88</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
       <c r="C19">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="D19">
         <v>160</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>4.875</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>88</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C20">
+        <v>62</v>
+      </c>
+      <c r="D20">
+        <v>160</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" ref="E20:E57" si="3">(C20/D20)*12</f>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G57" si="4">E20/2</f>
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="J20">
+        <v>88</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C21">
+        <v>85</v>
+      </c>
+      <c r="D21">
+        <v>160</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="3"/>
+        <v>6.375</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="4"/>
+        <v>3.1875</v>
+      </c>
+      <c r="J21">
+        <v>88</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>110</v>
+      </c>
+      <c r="D22">
+        <v>160</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="3"/>
+        <v>8.25</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="4"/>
+        <v>4.125</v>
+      </c>
+      <c r="J22">
+        <v>88</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>160</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="3"/>
+        <v>2.25</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="4"/>
+        <v>1.125</v>
+      </c>
+      <c r="J23">
+        <v>88</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>160</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="J24">
+        <v>88</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>160</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="3"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="4"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J25">
+        <v>88</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>160</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="J26">
+        <v>88</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>160</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="4"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J27">
+        <v>88</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>115</v>
+      </c>
+      <c r="D28">
+        <v>160</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="3"/>
+        <v>8.625</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="4"/>
+        <v>4.3125</v>
+      </c>
+      <c r="J28">
+        <v>88</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>160</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="J29">
+        <v>88</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>250</v>
+      </c>
+      <c r="D30">
+        <v>160</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>18.75</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="4"/>
+        <v>9.375</v>
+      </c>
+      <c r="J30">
+        <v>88</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C31">
+        <v>90</v>
+      </c>
+      <c r="D31">
+        <v>160</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="3"/>
+        <v>6.75</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="4"/>
+        <v>3.375</v>
+      </c>
+      <c r="J31">
+        <v>88</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>160</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>88</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>160</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="4"/>
+        <v>3.75</v>
+      </c>
+      <c r="J33">
+        <v>88</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>122</v>
+      </c>
+      <c r="D34">
+        <v>160</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="3"/>
+        <v>9.1499999999999986</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5749999999999993</v>
+      </c>
+      <c r="J34">
+        <v>88</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>160</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="4"/>
+        <v>1.875</v>
+      </c>
+      <c r="J35">
+        <v>88</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36">
+        <v>105</v>
+      </c>
+      <c r="D36">
+        <v>160</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="3"/>
+        <v>7.875</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="4"/>
+        <v>3.9375</v>
+      </c>
+      <c r="J36">
+        <v>88</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C37">
+        <v>80</v>
+      </c>
+      <c r="D37">
+        <v>160</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>88</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38">
+        <v>70</v>
+      </c>
+      <c r="D38">
+        <v>160</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="3"/>
+        <v>5.25</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="4"/>
+        <v>2.625</v>
+      </c>
+      <c r="J38">
+        <v>88</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>160</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="4"/>
+        <v>1.875</v>
+      </c>
+      <c r="J39">
+        <v>88</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <v>160</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="J40">
+        <v>150</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="2"/>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C41">
+        <v>220</v>
+      </c>
+      <c r="D41">
+        <v>160</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="3"/>
+        <v>16.5</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="4"/>
+        <v>8.25</v>
+      </c>
+      <c r="J41">
+        <v>88</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C42">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>160</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="4"/>
         <v>2.4375</v>
+      </c>
+      <c r="J42">
+        <v>88</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C43">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>160</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J43">
+        <v>88</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C44">
+        <v>65</v>
+      </c>
+      <c r="D44">
+        <v>160</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J44">
+        <v>88</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C45">
+        <v>65</v>
+      </c>
+      <c r="D45">
+        <v>160</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J45">
+        <v>88</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C46">
+        <v>65</v>
+      </c>
+      <c r="D46">
+        <v>160</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J46">
+        <v>88</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C47">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>160</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J47">
+        <v>88</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C48">
+        <v>65</v>
+      </c>
+      <c r="D48">
+        <v>160</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J48">
+        <v>88</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C49">
+        <v>65</v>
+      </c>
+      <c r="D49">
+        <v>160</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J49">
+        <v>88</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C50">
+        <v>65</v>
+      </c>
+      <c r="D50">
+        <v>160</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J50">
+        <v>88</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C51">
+        <v>65</v>
+      </c>
+      <c r="D51">
+        <v>160</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J51">
+        <v>88</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C52">
+        <v>65</v>
+      </c>
+      <c r="D52">
+        <v>160</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J52">
+        <v>88</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C53">
+        <v>65</v>
+      </c>
+      <c r="D53">
+        <v>160</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J53">
+        <v>88</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C54">
+        <v>65</v>
+      </c>
+      <c r="D54">
+        <v>160</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J54">
+        <v>88</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C55">
+        <v>65</v>
+      </c>
+      <c r="D55">
+        <v>160</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J55">
+        <v>88</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C56">
+        <v>65</v>
+      </c>
+      <c r="D56">
+        <v>160</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J56">
+        <v>88</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C57">
+        <v>65</v>
+      </c>
+      <c r="D57">
+        <v>160</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="3"/>
+        <v>4.875</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J57">
+        <v>88</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Ash Grove back height
</commit_message>
<xml_diff>
--- a/Pics/scale.xlsx
+++ b/Pics/scale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ModelRRProjects\AnyRail\Pics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A019843-6C7C-43A7-97AF-1FBA6D95CC0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B20421-7C8B-4F17-BD7A-D41E7733FDF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39910" yWindow="20070" windowWidth="16710" windowHeight="10340" xr2:uid="{F2CF72A6-85D0-419B-8904-BB52EA359DE2}"/>
+    <workbookView xWindow="38830" yWindow="7250" windowWidth="20690" windowHeight="21370" xr2:uid="{F2CF72A6-85D0-419B-8904-BB52EA359DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="AG" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>feet</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>Mill</t>
+  </si>
+  <si>
+    <t>DryPrep-Top</t>
+  </si>
+  <si>
+    <t>Klinker Storage</t>
+  </si>
+  <si>
+    <t>Twin Prep Storage</t>
+  </si>
+  <si>
+    <t>Twin Prep Top</t>
   </si>
 </sst>
 </file>
@@ -462,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC5BF58-5D6E-4D62-AD7B-B2BB68C10829}">
-  <dimension ref="B3:K57"/>
+  <dimension ref="B3:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,7 +507,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -521,96 +533,93 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="D5">
         <v>160</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E19" si="0">(C5/D5)*12</f>
-        <v>3.375</v>
+        <f>(C5/D5)*12</f>
+        <v>9.75</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G19" si="1">E5/2</f>
-        <v>1.6875</v>
+        <f>E5/2</f>
+        <v>4.875</v>
       </c>
       <c r="J5">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K57" si="2">(J5/D5)*12</f>
-        <v>6.6000000000000005</v>
+        <f>(J5/D5)*12</f>
+        <v>1.35</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
       <c r="C6">
-        <v>290</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>160</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>21.75</v>
+        <f>(C6/D6)*12</f>
+        <v>4.5</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>10.875</v>
-      </c>
-      <c r="J6">
-        <v>88</v>
+        <f>E6/2</f>
+        <v>2.25</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
+        <f>(J6/D6)*12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
       <c r="C7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>160</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <f t="shared" ref="E7:E8" si="0">(C7/D7)*12</f>
+        <v>1.35</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" ref="G7:G8" si="1">E7/2</f>
+        <v>0.67500000000000004</v>
       </c>
       <c r="J7">
         <v>88</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K7:K8" si="2">(J7/D7)*12</f>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C8">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>160</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>5.625</v>
+        <v>1.35</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>2.8125</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="J8">
         <v>88</v>
@@ -621,728 +630,728 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
       <c r="C9">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>160</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.52499999999999991</v>
+        <f t="shared" ref="E9:E23" si="3">(C9/D9)*12</f>
+        <v>3.375</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.26249999999999996</v>
+        <f t="shared" ref="G9:G23" si="4">E9/2</f>
+        <v>1.6875</v>
       </c>
       <c r="J9">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
+        <f t="shared" ref="K9:K61" si="5">(J9/D9)*12</f>
+        <v>14.25</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
       <c r="C10">
-        <v>68</v>
+        <v>290</v>
       </c>
       <c r="D10">
         <v>160</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>5.0999999999999996</v>
+        <f t="shared" si="3"/>
+        <v>21.75</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>2.5499999999999998</v>
+        <f t="shared" si="4"/>
+        <v>10.875</v>
       </c>
       <c r="J10">
         <v>88</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C11">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>160</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>3.5999999999999996</v>
+        <f t="shared" si="3"/>
+        <v>1.5</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999998</v>
+        <f t="shared" si="4"/>
+        <v>0.75</v>
       </c>
       <c r="J11">
         <v>88</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>160</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>9.75</v>
+        <f t="shared" si="3"/>
+        <v>5.625</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>4.875</v>
+        <f t="shared" si="4"/>
+        <v>2.8125</v>
       </c>
       <c r="J12">
         <v>88</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C13">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>160</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <f t="shared" si="3"/>
+        <v>0.52499999999999991</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
+        <f t="shared" si="4"/>
+        <v>0.26249999999999996</v>
       </c>
       <c r="J13">
         <v>88</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="C14">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>160</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="4"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J14">
+        <v>88</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <v>160</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="3"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="J15">
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>160</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E17" si="6">(C16/D16)*12</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G17" si="7">E16/2</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>140</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:K17" si="8">(J16/D16)*12</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>160</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>25</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="8"/>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C14">
+      <c r="C18">
         <v>42</v>
       </c>
-      <c r="D14">
-        <v>160</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
+      <c r="D18">
+        <v>160</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="3"/>
         <v>3.1500000000000004</v>
       </c>
-      <c r="G14" s="1">
-        <f t="shared" si="1"/>
+      <c r="G18" s="1">
+        <f t="shared" si="4"/>
         <v>1.5750000000000002</v>
       </c>
-      <c r="J14">
-        <v>88</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15">
-        <v>60</v>
-      </c>
-      <c r="D15">
-        <v>160</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="J15">
-        <v>88</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="C16">
-        <v>53</v>
-      </c>
-      <c r="D16">
-        <v>160</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>3.9749999999999996</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9874999999999998</v>
-      </c>
-      <c r="J16">
-        <v>88</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="C17">
-        <v>40</v>
-      </c>
-      <c r="D17">
-        <v>160</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="J17">
-        <v>88</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="C18">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>160</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="0"/>
-        <v>1.875</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>0.9375</v>
-      </c>
       <c r="J18">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
+        <f t="shared" si="5"/>
+        <v>7.875</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>160</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>4.5</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>2.25</v>
       </c>
       <c r="J19">
         <v>88</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C20">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D20">
         <v>160</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E20:E57" si="3">(C20/D20)*12</f>
-        <v>4.6500000000000004</v>
+        <f t="shared" si="3"/>
+        <v>3.9749999999999996</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ref="G20:G57" si="4">E20/2</f>
-        <v>2.3250000000000002</v>
+        <f t="shared" si="4"/>
+        <v>1.9874999999999998</v>
       </c>
       <c r="J20">
         <v>88</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C21">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>160</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="3"/>
-        <v>6.375</v>
+        <v>3</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="4"/>
-        <v>3.1875</v>
+        <v>1.5</v>
       </c>
       <c r="J21">
         <v>88</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
       <c r="C22">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <v>160</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="3"/>
-        <v>8.25</v>
+        <v>1.875</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="4"/>
-        <v>4.125</v>
+        <v>0.9375</v>
       </c>
       <c r="J22">
         <v>88</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
       <c r="C23">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="D23">
         <v>160</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="3"/>
-        <v>2.25</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="4"/>
-        <v>1.125</v>
+        <v>6</v>
       </c>
       <c r="J23">
         <v>88</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C24">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="D24">
         <v>160</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f t="shared" ref="E24:E61" si="9">(C24/D24)*12</f>
+        <v>4.6500000000000004</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
+        <f t="shared" ref="G24:G61" si="10">E24/2</f>
+        <v>2.3250000000000002</v>
       </c>
       <c r="J24">
         <v>88</v>
       </c>
       <c r="K24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C25">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="D25">
         <v>160</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="3"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" si="9"/>
+        <v>6.375</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="4"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="10"/>
+        <v>3.1875</v>
       </c>
       <c r="J25">
         <v>88</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D26">
         <v>160</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="3"/>
-        <v>0.89999999999999991</v>
+        <f t="shared" si="9"/>
+        <v>8.25</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="4"/>
-        <v>0.44999999999999996</v>
+        <f t="shared" si="10"/>
+        <v>4.125</v>
       </c>
       <c r="J26">
         <v>88</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C27">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>160</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="3"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" si="9"/>
+        <v>2.25</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="4"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="10"/>
+        <v>1.125</v>
       </c>
       <c r="J27">
         <v>88</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
       <c r="C28">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>160</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="3"/>
-        <v>8.625</v>
+        <f t="shared" si="9"/>
+        <v>1.5</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="4"/>
-        <v>4.3125</v>
+        <f t="shared" si="10"/>
+        <v>0.75</v>
       </c>
       <c r="J28">
         <v>88</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C29">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D29">
         <v>160</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f t="shared" si="9"/>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
+        <f t="shared" si="10"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="J29">
         <v>88</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="D30">
         <v>160</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="3"/>
-        <v>18.75</v>
+        <f t="shared" si="9"/>
+        <v>0.89999999999999991</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="4"/>
-        <v>9.375</v>
+        <f t="shared" si="10"/>
+        <v>0.44999999999999996</v>
       </c>
       <c r="J30">
         <v>88</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C31">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <v>160</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="3"/>
-        <v>6.75</v>
+        <f t="shared" si="9"/>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="4"/>
-        <v>3.375</v>
+        <f t="shared" si="10"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="J31">
         <v>88</v>
       </c>
       <c r="K31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D32">
         <v>160</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="9"/>
+        <v>8.625</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>4.3125</v>
       </c>
       <c r="J32">
         <v>88</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C33">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D33">
         <v>160</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="3"/>
-        <v>7.5</v>
+        <f t="shared" si="9"/>
+        <v>1.5</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="4"/>
-        <v>3.75</v>
+        <f t="shared" si="10"/>
+        <v>0.75</v>
       </c>
       <c r="J33">
         <v>88</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C34">
-        <v>122</v>
+        <v>250</v>
       </c>
       <c r="D34">
         <v>160</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="3"/>
-        <v>9.1499999999999986</v>
+        <f t="shared" si="9"/>
+        <v>18.75</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="4"/>
-        <v>4.5749999999999993</v>
+        <f t="shared" si="10"/>
+        <v>9.375</v>
       </c>
       <c r="J34">
         <v>88</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C35">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D35">
         <v>160</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="3"/>
-        <v>3.75</v>
+        <f t="shared" si="9"/>
+        <v>6.75</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="4"/>
-        <v>1.875</v>
+        <f t="shared" si="10"/>
+        <v>3.375</v>
       </c>
       <c r="J35">
         <v>88</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="D36">
         <v>160</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="3"/>
-        <v>7.875</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="4"/>
-        <v>3.9375</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
       </c>
       <c r="J36">
         <v>88</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C37">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D37">
         <v>160</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="9"/>
+        <v>7.5</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>3.75</v>
       </c>
       <c r="J37">
         <v>88</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C38">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="D38">
         <v>160</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="3"/>
-        <v>5.25</v>
+        <f t="shared" si="9"/>
+        <v>9.1499999999999986</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="4"/>
-        <v>2.625</v>
+        <f t="shared" si="10"/>
+        <v>4.5749999999999993</v>
       </c>
       <c r="J38">
         <v>88</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1354,159 +1363,165 @@
         <v>160</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.875</v>
       </c>
       <c r="J39">
         <v>88</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C40">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="D40">
         <v>160</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="9"/>
+        <v>7.875</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="4"/>
-        <v>1.5</v>
+        <f t="shared" si="10"/>
+        <v>3.9375</v>
       </c>
       <c r="J40">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
-        <v>11.25</v>
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C41">
-        <v>220</v>
+        <v>80</v>
       </c>
       <c r="D41">
         <v>160</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="3"/>
-        <v>16.5</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="4"/>
-        <v>8.25</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
       </c>
       <c r="J41">
         <v>88</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
       <c r="C42">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D42">
         <v>160</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="3"/>
-        <v>4.875</v>
+        <f t="shared" si="9"/>
+        <v>5.25</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="4"/>
-        <v>2.4375</v>
+        <f t="shared" si="10"/>
+        <v>2.625</v>
       </c>
       <c r="J42">
         <v>88</v>
       </c>
       <c r="K42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C43">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D43">
         <v>160</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="3"/>
-        <v>4.875</v>
+        <f t="shared" si="9"/>
+        <v>3.75</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="4"/>
-        <v>2.4375</v>
+        <f t="shared" si="10"/>
+        <v>1.875</v>
       </c>
       <c r="J43">
         <v>88</v>
       </c>
       <c r="K43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
       <c r="C44">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D44">
         <v>160</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="3"/>
-        <v>4.875</v>
+        <f t="shared" si="9"/>
+        <v>3</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="4"/>
-        <v>2.4375</v>
+        <f t="shared" si="10"/>
+        <v>1.5</v>
       </c>
       <c r="J44">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="K44">
-        <f t="shared" si="2"/>
-        <v>6.6000000000000005</v>
+        <f t="shared" si="5"/>
+        <v>11.25</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C45">
-        <v>65</v>
+        <v>220</v>
       </c>
       <c r="D45">
         <v>160</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="3"/>
-        <v>4.875</v>
+        <f t="shared" si="9"/>
+        <v>16.5</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="4"/>
-        <v>2.4375</v>
+        <f t="shared" si="10"/>
+        <v>8.25</v>
       </c>
       <c r="J45">
         <v>88</v>
       </c>
       <c r="K45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1518,18 +1533,18 @@
         <v>160</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J46">
         <v>88</v>
       </c>
       <c r="K46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1541,18 +1556,18 @@
         <v>160</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J47">
         <v>88</v>
       </c>
       <c r="K47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1564,18 +1579,18 @@
         <v>160</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J48">
         <v>88</v>
       </c>
       <c r="K48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1587,18 +1602,18 @@
         <v>160</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J49">
         <v>88</v>
       </c>
       <c r="K49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1610,18 +1625,18 @@
         <v>160</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J50">
         <v>88</v>
       </c>
       <c r="K50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1633,18 +1648,18 @@
         <v>160</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J51">
         <v>88</v>
       </c>
       <c r="K51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1656,18 +1671,18 @@
         <v>160</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J52">
         <v>88</v>
       </c>
       <c r="K52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1679,18 +1694,18 @@
         <v>160</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J53">
         <v>88</v>
       </c>
       <c r="K53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1702,18 +1717,18 @@
         <v>160</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J54">
         <v>88</v>
       </c>
       <c r="K54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1725,18 +1740,18 @@
         <v>160</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J55">
         <v>88</v>
       </c>
       <c r="K55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1748,18 +1763,18 @@
         <v>160</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J56">
         <v>88</v>
       </c>
       <c r="K56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -1771,18 +1786,110 @@
         <v>160</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.875</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2.4375</v>
       </c>
       <c r="J57">
         <v>88</v>
       </c>
       <c r="K57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <v>65</v>
+      </c>
+      <c r="D58">
+        <v>160</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="9"/>
+        <v>4.875</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J58">
+        <v>88</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>65</v>
+      </c>
+      <c r="D59">
+        <v>160</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="9"/>
+        <v>4.875</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J59">
+        <v>88</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>65</v>
+      </c>
+      <c r="D60">
+        <v>160</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="9"/>
+        <v>4.875</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J60">
+        <v>88</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="5"/>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>65</v>
+      </c>
+      <c r="D61">
+        <v>160</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="9"/>
+        <v>4.875</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J61">
+        <v>88</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="5"/>
         <v>6.6000000000000005</v>
       </c>
     </row>

</xml_diff>